<commit_message>
Connor: Updated experiment analysis and Dissertation.docx
</commit_message>
<xml_diff>
--- a/Documentation/Experiments/LoadBalancingApplication.xlsx
+++ b/Documentation/Experiments/LoadBalancingApplication.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="30">
   <si>
     <t>Run 1</t>
   </si>
@@ -106,6 +106,12 @@
   <si>
     <t>Load Balance 30 requests - pre-process (w/o load balancing) (3 instances of application)</t>
   </si>
+  <si>
+    <t>Percentage improvement in response time by scaling to 3 applications</t>
+  </si>
+  <si>
+    <t>Percentage improvement in  edge CPU use by scaling to 3 applications</t>
+  </si>
 </sst>
 </file>
 
@@ -172,11 +178,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -14756,7 +14762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB89"/>
   <sheetViews>
-    <sheetView topLeftCell="V25" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="AN51" sqref="AN51"/>
     </sheetView>
   </sheetViews>
@@ -15116,19 +15122,19 @@
       <c r="AB6" s="1"/>
     </row>
     <row r="7" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="10"/>
-      <c r="N7" s="9">
+      <c r="M7" s="9"/>
+      <c r="N7" s="10">
         <f>(L4-U4)/U4</f>
         <v>-1.1858132270054478E-3</v>
       </c>
-      <c r="P7" s="10" t="s">
+      <c r="P7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="9">
+      <c r="Q7" s="9"/>
+      <c r="R7" s="10">
         <f>(N4-W4)/W4</f>
         <v>1.0851162749896882E-2</v>
       </c>
@@ -15139,12 +15145,12 @@
       <c r="AB7" s="3"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="9"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="10"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="10"/>
       <c r="T8" s="5"/>
       <c r="U8" s="5"/>
       <c r="Z8" s="3"/>
@@ -15152,12 +15158,12 @@
       <c r="AB8" s="3"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="9"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="10"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="10"/>
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
       <c r="Z9" s="3"/>
@@ -20613,6 +20619,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B60:I60"/>
+    <mergeCell ref="K60:R60"/>
+    <mergeCell ref="T60:AA60"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="T2:AA2"/>
+    <mergeCell ref="R7:R9"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B76:I76"/>
     <mergeCell ref="K76:R76"/>
@@ -20629,13 +20642,6 @@
     <mergeCell ref="L7:M9"/>
     <mergeCell ref="N7:N9"/>
     <mergeCell ref="P7:Q9"/>
-    <mergeCell ref="B60:I60"/>
-    <mergeCell ref="K60:R60"/>
-    <mergeCell ref="T60:AA60"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="K2:R2"/>
-    <mergeCell ref="T2:AA2"/>
-    <mergeCell ref="R7:R9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -21006,19 +21012,19 @@
       <c r="AB6" s="4"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="10"/>
-      <c r="N7" s="9">
+      <c r="M7" s="9"/>
+      <c r="N7" s="10">
         <f>(L4-U4)/U4</f>
         <v>0.6120326755282377</v>
       </c>
-      <c r="P7" s="10" t="s">
+      <c r="P7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="9">
+      <c r="Q7" s="9"/>
+      <c r="R7" s="10">
         <f>(N4-W4)/W4</f>
         <v>1.9371228276165591E-2</v>
       </c>
@@ -21027,24 +21033,24 @@
       <c r="AB7" s="4"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="10"/>
       <c r="O8" s="7"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="10"/>
       <c r="Z8" s="4"/>
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="9"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="10"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="10"/>
       <c r="Z9" s="4"/>
       <c r="AA9" s="4"/>
       <c r="AB9" s="4"/>
@@ -26505,6 +26511,18 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B60:I60"/>
+    <mergeCell ref="K60:R60"/>
+    <mergeCell ref="T60:AA60"/>
+    <mergeCell ref="B76:I76"/>
+    <mergeCell ref="K76:R76"/>
+    <mergeCell ref="T76:AA76"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="K28:R28"/>
+    <mergeCell ref="T28:AA28"/>
+    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="K44:R44"/>
+    <mergeCell ref="T44:AA44"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="K2:R2"/>
@@ -26516,18 +26534,6 @@
     <mergeCell ref="N7:N9"/>
     <mergeCell ref="P7:Q9"/>
     <mergeCell ref="R7:R9"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="K28:R28"/>
-    <mergeCell ref="T28:AA28"/>
-    <mergeCell ref="B44:I44"/>
-    <mergeCell ref="K44:R44"/>
-    <mergeCell ref="T44:AA44"/>
-    <mergeCell ref="B60:I60"/>
-    <mergeCell ref="K60:R60"/>
-    <mergeCell ref="T60:AA60"/>
-    <mergeCell ref="B76:I76"/>
-    <mergeCell ref="K76:R76"/>
-    <mergeCell ref="T76:AA76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -26538,8 +26544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U52" workbookViewId="0">
-      <selection activeCell="AG96" sqref="AG96"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26898,45 +26904,45 @@
       <c r="AB6" s="6"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="L7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="10"/>
-      <c r="N7" s="9" t="e">
-        <f>(L4-U4)/U4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="9" t="e">
-        <f>(N4-W4)/W4</f>
-        <v>#DIV/0!</v>
+      <c r="L7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" s="9"/>
+      <c r="N7" s="10">
+        <f>('Load Balance 30'!L4-L4)/L4</f>
+        <v>1.2092194525345135</v>
+      </c>
+      <c r="P7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="10">
+        <f>('Load Balance 30'!N4-'Load Balance 30 3 instances'!N4)/'Load Balance 30 3 instances'!N4</f>
+        <v>0.26983158211716091</v>
       </c>
       <c r="Z7" s="6"/>
       <c r="AA7" s="6"/>
       <c r="AB7" s="6"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="10"/>
       <c r="O8" s="7"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="10"/>
       <c r="Z8" s="6"/>
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="9"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="10"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="10"/>
       <c r="Z9" s="6"/>
       <c r="AA9" s="6"/>
       <c r="AB9" s="6"/>
@@ -28101,7 +28107,7 @@
         <v>0.62241822309799022</v>
       </c>
       <c r="N41">
-        <f t="shared" ref="N41:Q41" si="10">STDEV(N30:N39)</f>
+        <f t="shared" ref="N41:P41" si="10">STDEV(N30:N39)</f>
         <v>8.1743403403577783</v>
       </c>
       <c r="O41">
@@ -29998,20 +30004,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="K2:R2"/>
-    <mergeCell ref="T2:AA2"/>
-    <mergeCell ref="L7:M9"/>
-    <mergeCell ref="N7:N9"/>
-    <mergeCell ref="P7:Q9"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="B12:I12"/>
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="T12:AA12"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="K28:R28"/>
-    <mergeCell ref="T28:AA28"/>
     <mergeCell ref="B76:I76"/>
     <mergeCell ref="K76:R76"/>
     <mergeCell ref="T76:AA76"/>
@@ -30021,6 +30013,20 @@
     <mergeCell ref="B60:I60"/>
     <mergeCell ref="K60:R60"/>
     <mergeCell ref="T60:AA60"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="T12:AA12"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="K28:R28"/>
+    <mergeCell ref="T28:AA28"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="T2:AA2"/>
+    <mergeCell ref="L7:M9"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="P7:Q9"/>
+    <mergeCell ref="R7:R9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>